<commit_message>
Update results & download some models
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D1099E-A356-9C4D-84F5-6D5A68B07F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675ECEC6-E65C-A44B-A00F-F788424A652A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="820" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
@@ -35,16 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>map9</t>
-  </si>
-  <si>
-    <t>map10</t>
-  </si>
-  <si>
-    <t>map11</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,10 +89,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>map8（朝左U形）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>稳的，快速通过</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -115,6 +102,70 @@
   </si>
   <si>
     <t>map7（圆形 终点在中间）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map9（L形）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map10（直角弯曲）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡墙，但相对来说走的远一些</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map11（弯曲加栏）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相对来说走的远一些</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>除了1基本都卡墙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不走Z字形了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有时能赢，仍会卡墙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>撞墙没有变少</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡墙严重</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use dist. reward + hit wall penalty (25) vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳，撞墙变少了一点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map8（朝左U形无箭头）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路线很曲折，走的不算远</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没跑？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -503,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -519,50 +570,52 @@
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="22.1640625" customWidth="1"/>
     <col min="8" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
         <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -579,29 +632,80 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update evaluation (add reverse)
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15AAFEE-BA5C-524A-A3ED-37C94CCF950B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E02F68A-2CBC-BE4E-8F0A-2BCE33062CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="820" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -349,7 +349,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PPO use step distance reward vs. Random</t>
+    <t>PPO use step distance reward + multiply critic lr + train every episode vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大力贴左墙</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -774,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -849,7 +853,9 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Update results & change main.py default argument
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEBD00C-EBF0-7245-98D4-05CC590CDC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD59E0E9-4012-0B43-9E36-116F5DCA3DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="820" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -349,11 +349,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PPO use step distance reward + multiply critic lr + train every episode vs. Random</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>大力贴左墙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use step distance reward + multiply critic lr + train every episode + MLP 3 frames vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run dir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_map*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_dist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_hit_wall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_hit_wall_[actor]_2layers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_summed_hit_wall_[MLP]_[frames]3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_hit_wall_[MLP]_[frames]3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_hit_wall_[MLP]_[frames]9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_hit_wall_[CNN]_[frames]3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_hit_wall_[CNN]_[frames]9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_summed_hit_wall_[MLP]_[frames]9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_step_dist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>反而是换边更顺，不过都还行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经常折返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不是稳赢，经常折返</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -778,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -796,6 +856,8 @@
     <col min="10" max="10" width="25.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="15" max="15" width="21.33203125" customWidth="1"/>
     <col min="16" max="16" width="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -842,6 +904,9 @@
       <c r="N1" t="s">
         <v>0</v>
       </c>
+      <c r="O1" t="s">
+        <v>80</v>
+      </c>
       <c r="P1" s="4" t="s">
         <v>56</v>
       </c>
@@ -854,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
@@ -869,6 +934,9 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
+      <c r="O2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="6" t="s">
@@ -911,6 +979,9 @@
       <c r="N3" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="O3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="6" t="s">
@@ -953,6 +1024,9 @@
       <c r="N4" t="s">
         <v>30</v>
       </c>
+      <c r="O4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="6" t="s">
@@ -985,6 +1059,9 @@
       <c r="M5" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="O5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="6" t="s">
@@ -1014,6 +1091,9 @@
       <c r="N6" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="O6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="6" t="s">
@@ -1040,6 +1120,9 @@
       <c r="M7" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="O7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="6" t="s">
@@ -1054,6 +1137,9 @@
       <c r="G8" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="O8" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="6" t="s">
@@ -1068,6 +1154,9 @@
       <c r="G9" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="O9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="6" t="s">
@@ -1082,6 +1171,9 @@
       <c r="I10" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="O10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="6" t="s">
@@ -1093,13 +1185,30 @@
       <c r="E11" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="O11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="J12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O13" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
download models & update results
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71C12A4-B735-9940-8D77-7BDF552C7BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99894018-B621-8E46-B4C7-D02D53CE0B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="820" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
+    <workbookView xWindow="1660" yWindow="1040" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -405,6 +405,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>map*_use_step_dist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>反而是换边更顺，不过都还行</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -421,7 +425,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>map*_use_step_dist，这个实际上是命错名了</t>
+    <t>map*_use_step_dist_[frames]3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只能过个弯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以，不流畅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经常走回头路，经常不过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经常走回头路，偶尔能过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>走的远一点，但是会卡角落</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只能过两三个弯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很标准沿中间走</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>偶尔折返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不是稳赢，经常折返+卡墙</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -846,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1197,14 +1241,6 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="J12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
     <row r="13" spans="1:16">
       <c r="A13" s="6" t="s">
         <v>77</v>
@@ -1212,19 +1248,61 @@
       <c r="B13" t="s">
         <v>78</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O13" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
         <v>80</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="O14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish some training & update results
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99894018-B621-8E46-B4C7-D02D53CE0B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911BEC49-A356-7D43-8871-CB045CB2349B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="1040" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="125">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -466,6 +466,74 @@
   </si>
   <si>
     <t>不是稳赢，经常折返+卡墙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD-N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use step distance reward + multiply critic lr + train every episode + normalized reward vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老大爷遛弯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对着墙跑，不怎么能移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡很久之后能过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完全不行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>转圈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四处碰壁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>转圈，上下碰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会折返很多，有时不能过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>即使快到了也要回去绕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>还算顺利</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not a chance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>受random干扰很大，但有一次居然靠自己过了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random没干扰就能过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>干扰很大，但是有时候能走的很远，几乎到终点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一开始卡半天，后来也只能过个弯</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -888,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1251,11 +1319,35 @@
       <c r="C13" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="J13" s="1" t="s">
         <v>106</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>107</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="O13" t="s">
         <v>92</v>
@@ -1303,6 +1395,45 @@
       </c>
       <c r="O14" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed config.json & download and update some results
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911BEC49-A356-7D43-8871-CB045CB2349B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7042DA86-B4FF-9447-B44C-C0110BF46D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="1040" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="132">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -534,6 +534,34 @@
   </si>
   <si>
     <t>一开始卡半天，后来也只能过个弯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD-SHW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use step distance reward + multiply critic lr + train every episode + summed hit wall penalty vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>走的不直线，所以有时输</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>撞墙还是不少</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>撞墙不多，但是有干扰的话就不知所措了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很强，马上就过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>受干扰的话可能寄</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -956,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="118" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1436,6 +1464,29 @@
         <v>115</v>
       </c>
     </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add options in main.py to control if train by win / train every episode
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7042DA86-B4FF-9447-B44C-C0110BF46D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0970CCA-8820-3747-924E-80032552E504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="1040" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="137">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -562,6 +562,26 @@
   </si>
   <si>
     <t>受干扰的话可能寄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use step distance reward + multiply critic lr + train every episode + summed hit wall penalty + actor 2 layers + 3 frames vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD-SHW-3F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_step_dist_normed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_step_dist_summed_hit_wall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_step_dist_summed_hit_wall_[actor]2layers_[frames]3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -984,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="118" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="87" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1005,7 +1025,7 @@
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.33203125" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" customWidth="1"/>
+    <col min="15" max="15" width="61.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1463,6 +1483,9 @@
       <c r="M15" s="2" t="s">
         <v>115</v>
       </c>
+      <c r="O15" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="6" t="s">
@@ -1485,6 +1508,20 @@
       </c>
       <c r="K16" s="1" t="s">
         <v>131</v>
+      </c>
+      <c r="O16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
+        <v>132</v>
+      </c>
+      <c r="O17" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "update some results"
This reverts commit 6003f15e27b7aee57d26b619ef043331a429dfc7.
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D992ED-44F8-324A-95F7-C63A1C3C3839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDF3529-8014-4B4A-96F8-4247CE725C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="1040" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="153">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -646,58 +646,6 @@
   </si>
   <si>
     <t>卡墙，很少能过</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>能过1 2 8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有时候折返能过1 2 8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>赢了15把，但是不太抗干扰，而且方式比较诡异</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>贴墙走</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在墙上弹几下</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map*_use_step_dist_self_play</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map*_use_dist_self_play</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SD-SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ED-SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PPO use episode distance reward + multiply critic lr + train every episode + self play vs. Random</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PPO use step distance reward + multiply critic lr + train every episode + self play vs. Random</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>过了好几个，1特别稳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>很快</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1120,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="82" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1702,55 +1650,6 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B20" t="s">
-        <v>163</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="O20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21" t="s">
-        <v>162</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="O21" t="s">
-        <v>159</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update results (best so far)
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D35BC-CF55-CB4B-8E23-E5DE9AE3D1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A23420F-D983-7644-B83A-396468FC8D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1040" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
+    <workbookView xWindow="1000" yWindow="4780" windowWidth="28580" windowHeight="13220" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="185">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -722,6 +722,58 @@
   </si>
   <si>
     <t>map*_use_dist_self_play_shuffle_pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并非稳赢，会折返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很稳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳的一匹，是目前最稳的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳的一匹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好稳啊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会贴墙，走的太慢了，不过还是蛮远的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并非稳赢，有时卡墙or折返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>甚至好像学会了堵路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>到不了最上面一层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进不去</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED-SP-Spos-3F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use episode distance reward + multiply critic lr + train every episode + self play + shuffle position + actor 2 layers + 3 frames vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打Baseline或random的冲线率都是65%，跟baseline打rewar的胜率是甚至各把11给过了一次！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1144,10 +1196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1782,6 +1834,12 @@
       <c r="B22" t="s">
         <v>167</v>
       </c>
+      <c r="H22" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>181</v>
+      </c>
       <c r="O22" t="s">
         <v>170</v>
       </c>
@@ -1793,8 +1851,52 @@
       <c r="B23" t="s">
         <v>169</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>184</v>
+      </c>
       <c r="O23" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Update results (best so far)"
This reverts commit 79d0814e21cc43a9dbd796e7cda25bf1f55311a5.
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A23420F-D983-7644-B83A-396468FC8D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D35BC-CF55-CB4B-8E23-E5DE9AE3D1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="4780" windowWidth="28580" windowHeight="13220" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
+    <workbookView xWindow="1660" yWindow="1040" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="172">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -722,58 +722,6 @@
   </si>
   <si>
     <t>map*_use_dist_self_play_shuffle_pos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>并非稳赢，会折返</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>很稳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>稳的一匹，是目前最稳的</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>稳的一匹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>好稳啊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>会贴墙，走的太慢了，不过还是蛮远的</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>并非稳赢，有时卡墙or折返</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>甚至好像学会了堵路</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>到不了最上面一层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>进不去</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ED-SP-Spos-3F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PPO use episode distance reward + multiply critic lr + train every episode + self play + shuffle position + actor 2 layers + 3 frames vs. Random</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>打Baseline或random的冲线率都是65%，跟baseline打rewar的胜率是甚至各把11给过了一次！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1196,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="I2" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1834,12 +1782,6 @@
       <c r="B22" t="s">
         <v>167</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="O22" t="s">
         <v>170</v>
       </c>
@@ -1851,52 +1793,8 @@
       <c r="B23" t="s">
         <v>169</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="O23" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B24" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Update results (best so far)""
This reverts commit 656e593f09fe922a38920e1f6bc756b9635a091d.
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D35BC-CF55-CB4B-8E23-E5DE9AE3D1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A23420F-D983-7644-B83A-396468FC8D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1040" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
+    <workbookView xWindow="1000" yWindow="4780" windowWidth="28580" windowHeight="13220" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="185">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -722,6 +722,58 @@
   </si>
   <si>
     <t>map*_use_dist_self_play_shuffle_pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并非稳赢，会折返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很稳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳的一匹，是目前最稳的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳的一匹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好稳啊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会贴墙，走的太慢了，不过还是蛮远的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并非稳赢，有时卡墙or折返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>甚至好像学会了堵路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>到不了最上面一层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进不去</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED-SP-Spos-3F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use episode distance reward + multiply critic lr + train every episode + self play + shuffle position + actor 2 layers + 3 frames vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打Baseline或random的冲线率都是65%，跟baseline打rewar的胜率是甚至各把11给过了一次！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1144,10 +1196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1782,6 +1834,12 @@
       <c r="B22" t="s">
         <v>167</v>
       </c>
+      <c r="H22" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>181</v>
+      </c>
       <c r="O22" t="s">
         <v>170</v>
       </c>
@@ -1793,8 +1851,52 @@
       <c r="B23" t="s">
         <v>169</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>184</v>
+      </c>
       <c r="O23" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "update results""
This reverts commit dfb17280621c5b6cfd692039d8f5b5c0284607a4.
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A23420F-D983-7644-B83A-396468FC8D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B97591-5FC3-FD40-8575-055738263ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="4780" windowWidth="28580" windowHeight="13220" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
+    <workbookView xWindow="30860" yWindow="1640" windowWidth="36200" windowHeight="18120" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="187">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -774,6 +774,14 @@
   </si>
   <si>
     <t>打Baseline或random的冲线率都是65%，跟baseline打rewar的胜率是甚至各把11给过了一次！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_dist_self_play_shuffle_pos_[actor]2layers_[frames]3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1198,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="133" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1898,6 +1906,18 @@
       <c r="B24" t="s">
         <v>183</v>
       </c>
+      <c r="H24" t="s">
+        <v>185</v>
+      </c>
+      <c r="M24" t="s">
+        <v>185</v>
+      </c>
+      <c r="N24" t="s">
+        <v>185</v>
+      </c>
+      <c r="O24" t="s">
+        <v>186</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Fix bugs in evaluation
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDF3529-8014-4B4A-96F8-4247CE725C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C7B667-DBEB-FC4A-B282-852EA330269E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1040" windowWidth="28220" windowHeight="17440" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
+    <workbookView xWindow="30860" yWindow="1640" windowWidth="36200" windowHeight="18120" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="189">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -646,6 +646,150 @@
   </si>
   <si>
     <t>卡墙，很少能过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>能过1 2 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有时候折返能过1 2 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赢了15把，但是不太抗干扰，而且方式比较诡异</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贴墙走</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在墙上弹几下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_step_dist_self_play</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_dist_self_play</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD-SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED-SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use episode distance reward + multiply critic lr + train every episode + self play vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use step distance reward + multiply critic lr + train every episode + self play vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>过了好几个，1特别稳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很快</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD-SP-Spos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use step distance reward + multiply critic lr + train every episode + self play + shuffle position vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED-SP-Spos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use episode distance reward + multiply critic lr + train every episode + self play + shuffle position vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_step_dist_self_play_shuffle_pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_dist_self_play_shuffle_pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并非稳赢，会折返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很稳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳的一匹，是目前最稳的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳的一匹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好稳啊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会贴墙，走的太慢了，不过还是蛮远的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并非稳赢，有时卡墙or折返</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>甚至好像学会了堵路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>到不了最上面一层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进不去</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED-SP-Spos-3F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use episode distance reward + multiply critic lr + train every episode + self play + shuffle position + actor 2 layers + 3 frames vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打Baseline或random的冲线率都是65%，跟baseline打rewar的胜率是甚至各把11给过了一次！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map*_use_dist_self_play_shuffle_pos_[actor]2layers_[frames]3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>懒得一批</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>转圈且行动缓慢</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1068,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="82" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="117" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1650,6 +1794,139 @@
         <v>139</v>
       </c>
     </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="O20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="O21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="O22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="O23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
+      <c r="H24" t="s">
+        <v>185</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="O24" t="s">
+        <v>186</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bug fix in evaluation & main
</commit_message>
<xml_diff>
--- a/实验结果记录.xlsx
+++ b/实验结果记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cantabile/Desktop/学期文件/大三下/博弈论与多智能体学习/OlympicsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C7B667-DBEB-FC4A-B282-852EA330269E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E065290C-2855-7E44-9ED2-CBA678818704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30860" yWindow="1640" windowWidth="36200" windowHeight="18120" xr2:uid="{CE1DCB75-E044-ED49-867C-1A849C5460CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="194">
   <si>
     <t>all</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -790,6 +790,26 @@
   </si>
   <si>
     <t>转圈且行动缓慢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use episode distance reward + multiply critic lr + train every episode + self play + shuffle position + CNN + big batch + use cross  vs. Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>转圈，估计一个都过不了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED-SP-Spos-CNN-BB-Crs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED-SP-Spos-MLP-BB-Crs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO use episode distance reward + multiply critic lr + train every episode + self play + shuffle position + MLP (actor 2 layers) + big batch + use cross  vs. Random</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1212,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D212FD-EE9D-944D-9274-9E6E30EF71E0}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="117" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1927,6 +1947,25 @@
         <v>186</v>
       </c>
     </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" t="s">
+        <v>189</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" t="s">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>